<commit_message>
ajout des page pour le mdp
</commit_message>
<xml_diff>
--- a/Projet final/traitement/Commandes_Snack.xlsx
+++ b/Projet final/traitement/Commandes_Snack.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>NOM</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>NAKHIL</t>
+  </si>
+  <si>
+    <t>Amine</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
   <si>
     <t>Total VIANDE</t>
@@ -396,7 +405,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,7 +440,26 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -466,19 +494,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -489,13 +517,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>